<commit_message>
update with consomation and production function
</commit_message>
<xml_diff>
--- a/projet/Spherodisation/Transitoire/Resultats.xlsx
+++ b/projet/Spherodisation/Transitoire/Resultats.xlsx
@@ -746,31 +746,31 @@
         <v>1250</v>
       </c>
       <c r="B9" t="n">
-        <v>3000</v>
+        <v>1250</v>
       </c>
       <c r="C9" t="n">
-        <v>800</v>
+        <v>1250</v>
       </c>
       <c r="D9" t="n">
         <v/>
       </c>
       <c r="E9" t="n">
-        <v>0.0625517855946397</v>
+        <v>0.05</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02328657733109998</v>
+        <v>0.05</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1004146649916249</v>
+        <v>0.05</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0625517855946397</v>
+        <v>0.045</v>
       </c>
       <c r="I9" t="n">
-        <v>0.03474318007685483</v>
+        <v>0.0425</v>
       </c>
       <c r="J9" t="n">
-        <v>0.04500038707788115</v>
+        <v>0.045</v>
       </c>
     </row>
     <row r="10">
@@ -855,7 +855,7 @@
         <v/>
       </c>
       <c r="E12" t="n">
-        <v>22.04223240502277</v>
+        <v>17.93196593785158</v>
       </c>
       <c r="F12" t="n">
         <v/>

</xml_diff>